<commit_message>
MessagingCore: Update RuleSets.fsh fdd883ac202233b79b529aad4f9b469b39a4fc4a
</commit_message>
<xml_diff>
--- a/igs/MessagingCore/StructureDefinition-HopsMessageHeader.xlsx
+++ b/igs/MessagingCore/StructureDefinition-HopsMessageHeader.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$73</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2474" uniqueCount="404">
   <si>
     <t>Path</t>
   </si>
@@ -1047,34 +1047,7 @@
     <t>MessageHeader.response.extension</t>
   </si>
   <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
     <t>MessageHeader.response.modifierExtension</t>
-  </si>
-  <si>
-    <t>extensions
-user contentmodifiers</t>
-  </si>
-  <si>
-    <t>Extensions that cannot be ignored even if unrecognized</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
-Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
-  </si>
-  <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>MessageHeader.response.identifier</t>
@@ -1147,6 +1120,93 @@
     <t>AcknowledgementDetail or Observation[classCode="ALRT" and moodCode="EVN"]</t>
   </si>
   <si>
+    <t>MessageHeader.response.details.id</t>
+  </si>
+  <si>
+    <t>MessageHeader.response.details.extension</t>
+  </si>
+  <si>
+    <t>MessageHeader.response.details.reference</t>
+  </si>
+  <si>
+    <t>Literal reference, Relative, internal or absolute URL</t>
+  </si>
+  <si>
+    <t>A reference to a location at which the other resource is found. The reference may be a relative reference, in which case it is relative to the service base URL, or an absolute URL that resolves to the location where the resource is found. The reference may be version specific or not. If the reference is not to a FHIR RESTful server, then it should be assumed to be version specific. Internal fragment references (start with '#') refer to contained resources.</t>
+  </si>
+  <si>
+    <t>Using absolute URLs provides a stable scalable approach suitable for a cloud/web context, while using relative/logical references provides a flexible approach suitable for use when trading across closed eco-system boundaries.   Absolute URLs do not need to point to a FHIR RESTful server, though this is the preferred approach. If the URL conforms to the structure "/[type]/[id]" then it should be assumed that the reference is to a FHIR RESTful server.</t>
+  </si>
+  <si>
+    <t>Reference.reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref-1
+</t>
+  </si>
+  <si>
+    <t>MessageHeader.response.details.type</t>
+  </si>
+  <si>
+    <t>Type the reference refers to (e.g. "Patient")</t>
+  </si>
+  <si>
+    <t>The expected type of the target of the reference. If both Reference.type and Reference.reference are populated and Reference.reference is a FHIR URL, both SHALL be consistent.
+The type is the Canonical URL of Resource Definition that is the type this reference refers to. References are URLs that are relative to http://hl7.org/fhir/StructureDefinition/ e.g. "Patient" is a reference to http://hl7.org/fhir/StructureDefinition/Patient. Absolute URLs are only allowed for logical models (and can only be used in references in logical models, not resources).</t>
+  </si>
+  <si>
+    <t>This element is used to indicate the type of  the target of the reference. This may be used which ever of the other elements are populated (or not). In some cases, the type of the target may be determined by inspection of the reference (e.g. a RESTful URL) or by resolving the target of the reference; if both the type and a reference is provided, the reference SHALL resolve to a resource of the same type as that specified.</t>
+  </si>
+  <si>
+    <t>Aa resource (or, for logical models, the URI of the logical model).</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/resource-types</t>
+  </si>
+  <si>
+    <t>Reference.type</t>
+  </si>
+  <si>
+    <t>MessageHeader.response.details.identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier
+</t>
+  </si>
+  <si>
+    <t>Logical reference, when literal reference is not known</t>
+  </si>
+  <si>
+    <t>An identifier for the target resource. This is used when there is no way to reference the other resource directly, either because the entity it represents is not available through a FHIR server, or because there is no way for the author of the resource to convert a known identifier to an actual location. There is no requirement that a Reference.identifier point to something that is actually exposed as a FHIR instance, but it SHALL point to a business concept that would be expected to be exposed as a FHIR instance, and that instance would need to be of a FHIR resource type allowed by the reference.</t>
+  </si>
+  <si>
+    <t>When an identifier is provided in place of a reference, any system processing the reference will only be able to resolve the identifier to a reference if it understands the business context in which the identifier is used. Sometimes this is global (e.g. a national identifier) but often it is not. For this reason, none of the useful mechanisms described for working with references (e.g. chaining, includes) are possible, nor should servers be expected to be able resolve the reference. Servers may accept an identifier based reference untouched, resolve it, and/or reject it - see CapabilityStatement.rest.resource.referencePolicy. 
+When both an identifier and a literal reference are provided, the literal reference is preferred. Applications processing the resource are allowed - but not required - to check that the identifier matches the literal reference
+Applications converting a logical reference to a literal reference may choose to leave the logical reference present, or remove it.
+Reference is intended to point to a structure that can potentially be expressed as a FHIR resource, though there is no need for it to exist as an actual FHIR resource instance - except in as much as an application wishes to actual find the target of the reference. The content referred to be the identifier must meet the logical constraints implied by any limitations on what resource types are permitted for the reference.  For example, it would not be legitimate to send the identifier for a drug prescription if the type were Reference(Observation|DiagnosticReport).  One of the use-cases for Reference.identifier is the situation where no FHIR representation exists (where the type is Reference (Any).</t>
+  </si>
+  <si>
+    <t>Reference.identifier</t>
+  </si>
+  <si>
+    <t>.identifier</t>
+  </si>
+  <si>
+    <t>MessageHeader.response.details.display</t>
+  </si>
+  <si>
+    <t>Text alternative for the resource</t>
+  </si>
+  <si>
+    <t>Plain text narrative that identifies the resource in addition to the resource reference.</t>
+  </si>
+  <si>
+    <t>This is generally not the same as the Resource.text of the referenced resource.  The purpose is to identify what's being referenced, not to fully describe it.</t>
+  </si>
+  <si>
+    <t>Reference.display</t>
+  </si>
+  <si>
     <t>MessageHeader.focus</t>
   </si>
   <si>
@@ -1167,6 +1227,24 @@
   </si>
   <si>
     <t>unique(./controlAct[classCode="CACT" and classCode="EVN" and isNormalAct()]/participation[typeCode="SUBJ" and isNormalParticipation]/role or ./controlAct[classCode="CACT" and classCode="EVN" and isNormalAct()]/outboundRelationship[typeCode="SBJ" and isNormalActRelatoinship]/target)</t>
+  </si>
+  <si>
+    <t>MessageHeader.focus.id</t>
+  </si>
+  <si>
+    <t>MessageHeader.focus.extension</t>
+  </si>
+  <si>
+    <t>MessageHeader.focus.reference</t>
+  </si>
+  <si>
+    <t>MessageHeader.focus.type</t>
+  </si>
+  <si>
+    <t>MessageHeader.focus.identifier</t>
+  </si>
+  <si>
+    <t>MessageHeader.focus.display</t>
   </si>
   <si>
     <t>MessageHeader.definition</t>
@@ -1334,7 +1412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL61"/>
+  <dimension ref="A1:AL73"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -7112,7 +7190,7 @@
         <v>40</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>39</v>
@@ -7211,14 +7289,14 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>334</v>
+        <v>39</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F55" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G55" t="s" s="2">
         <v>39</v>
@@ -7233,14 +7311,12 @@
         <v>67</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>335</v>
+        <v>68</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>337</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
         <v>39</v>
@@ -7307,7 +7383,7 @@
         <v>39</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>39</v>
@@ -7315,18 +7391,18 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>339</v>
+        <v>39</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>39</v>
@@ -7341,17 +7417,13 @@
         <v>67</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>340</v>
+        <v>68</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>342</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
         <v>39</v>
       </c>
@@ -7417,7 +7489,7 @@
         <v>39</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>147</v>
+        <v>39</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>39</v>
@@ -7425,7 +7497,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7451,14 +7523,14 @@
         <v>76</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" t="s" s="2">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>39</v>
@@ -7507,7 +7579,7 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>48</v>
@@ -7522,10 +7594,10 @@
         <v>60</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>39</v>
@@ -7533,7 +7605,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7559,16 +7631,16 @@
         <v>122</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>39</v>
@@ -7596,10 +7668,10 @@
         <v>143</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>39</v>
@@ -7617,7 +7689,7 @@
         <v>39</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>48</v>
@@ -7632,10 +7704,10 @@
         <v>60</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>39</v>
@@ -7643,7 +7715,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7666,19 +7738,19 @@
         <v>49</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>39</v>
@@ -7727,7 +7799,7 @@
         <v>39</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7742,10 +7814,10 @@
         <v>60</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>39</v>
@@ -7753,7 +7825,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7764,7 +7836,7 @@
         <v>40</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>39</v>
@@ -7773,23 +7845,19 @@
         <v>39</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>367</v>
+        <v>50</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>368</v>
+        <v>62</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>371</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>39</v>
       </c>
@@ -7837,25 +7905,25 @@
         <v>39</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>366</v>
+        <v>64</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>372</v>
+        <v>65</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>39</v>
@@ -7863,7 +7931,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -7883,21 +7951,19 @@
         <v>39</v>
       </c>
       <c r="I61" t="s" s="2">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>374</v>
+        <v>67</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>375</v>
+        <v>68</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>376</v>
+        <v>69</v>
       </c>
       <c r="M61" s="2"/>
-      <c r="N61" t="s" s="2">
-        <v>377</v>
-      </c>
+      <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>39</v>
       </c>
@@ -7933,44 +7999,1338 @@
         <v>39</v>
       </c>
       <c r="AA61" t="s" s="2">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="AB61" t="s" s="2">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="AC61" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD61" t="s" s="2">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="AE61" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" hidden="true">
+      <c r="A62" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="F62" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I62" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J62" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="N62" s="2"/>
+      <c r="O62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P62" s="2"/>
+      <c r="Q62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="AF62" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG62" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH62" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AL62" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" hidden="true">
+      <c r="A63" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F63" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I63" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J63" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K63" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="L63" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="M63" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="N63" s="2"/>
+      <c r="O63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P63" s="2"/>
+      <c r="Q63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W63" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="X63" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="Y63" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="Z63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE63" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="AF63" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG63" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI63" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ63" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK63" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AL63" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" hidden="true">
+      <c r="A64" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="AF61" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG61" t="s" s="2">
+      <c r="B64" s="2"/>
+      <c r="C64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F64" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I64" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J64" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="K64" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="L64" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="N64" s="2"/>
+      <c r="O64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P64" s="2"/>
+      <c r="Q64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE64" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="AF64" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG64" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="AH61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI61" t="s" s="2">
+      <c r="AH64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI64" t="s" s="2">
         <v>60</v>
       </c>
-      <c r="AJ61" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AK61" t="s" s="2">
+      <c r="AJ64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="AL64" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" hidden="true">
+      <c r="A65" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F65" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I65" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J65" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="K65" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="L65" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="M65" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="N65" s="2"/>
+      <c r="O65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P65" s="2"/>
+      <c r="Q65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE65" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AF65" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG65" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI65" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AL65" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" hidden="true">
+      <c r="A66" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F66" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I66" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J66" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="K66" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L66" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="N66" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="O66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P66" s="2"/>
+      <c r="Q66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="AF66" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG66" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI66" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="AL66" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" hidden="true">
+      <c r="A67" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F67" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J67" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="K67" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="L67" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P67" s="2"/>
+      <c r="Q67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE67" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AF67" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG67" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK67" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="AL67" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" hidden="true">
+      <c r="A68" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F68" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J68" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="K68" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="L68" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P68" s="2"/>
+      <c r="Q68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA68" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AB68" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD68" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AE68" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF68" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG68" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI68" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL68" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" hidden="true">
+      <c r="A69" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="F69" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I69" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J69" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="K69" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="L69" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="N69" s="2"/>
+      <c r="O69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P69" s="2"/>
+      <c r="Q69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE69" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="AF69" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG69" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH69" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="AI69" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK69" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AL69" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" hidden="true">
+      <c r="A70" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F70" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I70" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J70" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K70" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="L70" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="M70" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="N70" s="2"/>
+      <c r="O70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P70" s="2"/>
+      <c r="Q70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W70" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="X70" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="Y70" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="Z70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE70" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="AF70" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG70" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI70" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK70" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AL70" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" hidden="true">
+      <c r="A71" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F71" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I71" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J71" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="K71" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="L71" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="M71" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="N71" s="2"/>
+      <c r="O71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P71" s="2"/>
+      <c r="Q71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE71" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="AL61" t="s" s="2">
+      <c r="AF71" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG71" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI71" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ71" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK71" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="AL71" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" hidden="true">
+      <c r="A72" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F72" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I72" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J72" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="K72" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="L72" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="M72" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="N72" s="2"/>
+      <c r="O72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P72" s="2"/>
+      <c r="Q72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE72" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AF72" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG72" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI72" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK72" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AL72" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" hidden="true">
+      <c r="A73" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F73" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I73" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J73" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="K73" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="L73" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="M73" s="2"/>
+      <c r="N73" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="O73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P73" s="2"/>
+      <c r="Q73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE73" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="AF73" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG73" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI73" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AJ73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK73" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AL73" t="s" s="2">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL61">
+  <autoFilter ref="A1:AL73">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7980,7 +9340,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI60">
+  <conditionalFormatting sqref="A2:AI72">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
MessagingCore: her-id invariant 80a34709268e53c4c44c34103da2aa23153d78d2
</commit_message>
<xml_diff>
--- a/igs/MessagingCore/StructureDefinition-HopsMessageHeader.xlsx
+++ b/igs/MessagingCore/StructureDefinition-HopsMessageHeader.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2474" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2474" uniqueCount="406">
   <si>
     <t>Path</t>
   </si>
@@ -184,7 +184,7 @@
     <t>Resource.id</t>
   </si>
   <si>
-    <t xml:space="preserve">valid-uuid:Must be a valid uuid {$this.matches('[0-9a-f]{8}-[0-9a-f]{4}-[0-9a-f]{4}-[0-9a-f]{4}-[0-9a-f]{12}')}
+    <t xml:space="preserve">valid-uuid:Must be a valid uuid {$this.matches('^[0-9a-f]{8}-[0-9a-f]{4}-[0-9a-f]{4}-[0-9a-f]{4}-[0-9a-f]{12}$')}
 </t>
   </si>
   <si>
@@ -781,6 +781,10 @@
   </si>
   <si>
     <t>Identifies where to route the message.</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+valid-her-id:Must be a valid HER-ID prefixed with OID namespace: urn:oid:2.16.578.1.12.4.1.2.{id} {$this.matches('^urn:oid:2\.16\.578\.1\.12\.4\.1\.2\.[1-9][0-9]{0,7}$')}</t>
   </si>
   <si>
     <t>MSH-25 (or MSH-6)</t>
@@ -5439,13 +5443,13 @@
         <v>39</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>61</v>
+        <v>247</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>39</v>
@@ -5453,7 +5457,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5476,17 +5480,17 @@
         <v>49</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>39</v>
@@ -5535,7 +5539,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5550,10 +5554,10 @@
         <v>61</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>224</v>
@@ -5561,7 +5565,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5584,19 +5588,19 @@
         <v>49</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>39</v>
@@ -5645,7 +5649,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5660,10 +5664,10 @@
         <v>61</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>224</v>
@@ -5671,7 +5675,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5694,19 +5698,19 @@
         <v>49</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>39</v>
@@ -5755,7 +5759,7 @@
         <v>39</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5770,18 +5774,18 @@
         <v>61</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5804,19 +5808,19 @@
         <v>49</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>39</v>
@@ -5865,7 +5869,7 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -5880,18 +5884,18 @@
         <v>61</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5917,14 +5921,14 @@
         <v>218</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>39</v>
@@ -5973,7 +5977,7 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>48</v>
@@ -5991,15 +5995,15 @@
         <v>39</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6105,7 +6109,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6211,7 +6215,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6317,7 +6321,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6346,11 +6350,11 @@
         <v>230</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>39</v>
@@ -6399,7 +6403,7 @@
         <v>39</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
@@ -6414,10 +6418,10 @@
         <v>61</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>39</v>
@@ -6425,7 +6429,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6451,14 +6455,14 @@
         <v>50</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>39</v>
@@ -6507,7 +6511,7 @@
         <v>39</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6522,10 +6526,10 @@
         <v>61</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>39</v>
@@ -6533,7 +6537,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6559,14 +6563,14 @@
         <v>50</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>39</v>
@@ -6615,7 +6619,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6630,10 +6634,10 @@
         <v>61</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>39</v>
@@ -6641,7 +6645,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6664,17 +6668,17 @@
         <v>49</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>39</v>
@@ -6723,7 +6727,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6738,10 +6742,10 @@
         <v>61</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>39</v>
@@ -6749,7 +6753,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6775,16 +6779,16 @@
         <v>242</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>245</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>39</v>
@@ -6833,7 +6837,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>48</v>
@@ -6848,10 +6852,10 @@
         <v>61</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>39</v>
@@ -6859,7 +6863,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6882,19 +6886,19 @@
         <v>49</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>39</v>
@@ -6943,7 +6947,7 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -6958,18 +6962,18 @@
         <v>61</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -6992,17 +6996,17 @@
         <v>49</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>39</v>
@@ -7030,10 +7034,10 @@
         <v>113</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>39</v>
@@ -7051,7 +7055,7 @@
         <v>39</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7066,18 +7070,18 @@
         <v>61</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7103,10 +7107,10 @@
         <v>218</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7157,7 +7161,7 @@
         <v>39</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>40</v>
@@ -7172,10 +7176,10 @@
         <v>61</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>39</v>
@@ -7183,7 +7187,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7289,7 +7293,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7395,7 +7399,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7501,7 +7505,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7527,14 +7531,14 @@
         <v>77</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>39</v>
@@ -7583,7 +7587,7 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>48</v>
@@ -7598,10 +7602,10 @@
         <v>61</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>39</v>
@@ -7609,7 +7613,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7635,16 +7639,16 @@
         <v>123</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>39</v>
@@ -7672,10 +7676,10 @@
         <v>144</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>39</v>
@@ -7693,7 +7697,7 @@
         <v>39</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>48</v>
@@ -7708,10 +7712,10 @@
         <v>61</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>39</v>
@@ -7719,7 +7723,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7742,19 +7746,19 @@
         <v>49</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>39</v>
@@ -7803,7 +7807,7 @@
         <v>39</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7818,10 +7822,10 @@
         <v>61</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>39</v>
@@ -7829,7 +7833,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7935,7 +7939,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8041,7 +8045,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8067,13 +8071,13 @@
         <v>50</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8123,7 +8127,7 @@
         <v>39</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8132,7 +8136,7 @@
         <v>48</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AI62" t="s" s="2">
         <v>61</v>
@@ -8149,7 +8153,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8175,13 +8179,13 @@
         <v>89</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -8210,10 +8214,10 @@
         <v>105</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="Z63" t="s" s="2">
         <v>39</v>
@@ -8231,7 +8235,7 @@
         <v>39</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8257,7 +8261,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8280,16 +8284,16 @@
         <v>49</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8339,7 +8343,7 @@
         <v>39</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
@@ -8357,7 +8361,7 @@
         <v>39</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>39</v>
@@ -8365,7 +8369,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8391,13 +8395,13 @@
         <v>50</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
@@ -8447,7 +8451,7 @@
         <v>39</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>40</v>
@@ -8473,7 +8477,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8496,19 +8500,19 @@
         <v>49</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>39</v>
@@ -8557,7 +8561,7 @@
         <v>39</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>40</v>
@@ -8575,7 +8579,7 @@
         <v>39</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>39</v>
@@ -8583,7 +8587,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8689,7 +8693,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8795,7 +8799,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8821,13 +8825,13 @@
         <v>50</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
@@ -8877,7 +8881,7 @@
         <v>39</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>40</v>
@@ -8886,7 +8890,7 @@
         <v>48</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>61</v>
@@ -8903,7 +8907,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -8929,13 +8933,13 @@
         <v>89</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
@@ -8964,10 +8968,10 @@
         <v>105</v>
       </c>
       <c r="X70" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="Y70" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>39</v>
@@ -8985,7 +8989,7 @@
         <v>39</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>40</v>
@@ -9011,7 +9015,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9034,16 +9038,16 @@
         <v>49</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
@@ -9093,7 +9097,7 @@
         <v>39</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>40</v>
@@ -9111,7 +9115,7 @@
         <v>39</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>39</v>
@@ -9119,7 +9123,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9145,13 +9149,13 @@
         <v>50</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
@@ -9201,7 +9205,7 @@
         <v>39</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>40</v>
@@ -9227,7 +9231,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9250,17 +9254,17 @@
         <v>49</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>39</v>
@@ -9309,7 +9313,7 @@
         <v>39</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>40</v>
@@ -9327,7 +9331,7 @@
         <v>39</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>39</v>

</xml_diff>

<commit_message>
MessagingCore: added her-id example 7f4503f1dcd061c58fa5e0c05e43a36f7fd18a14
</commit_message>
<xml_diff>
--- a/igs/MessagingCore/StructureDefinition-HopsMessageHeader.xlsx
+++ b/igs/MessagingCore/StructureDefinition-HopsMessageHeader.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2474" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2474" uniqueCount="407">
   <si>
     <t>Path</t>
   </si>
@@ -783,8 +783,11 @@
     <t>Identifies where to route the message.</t>
   </si>
   <si>
+    <t>urn:oid:2.16.578.1.12.4.1.2.131725</t>
+  </si>
+  <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-valid-her-id:Must be a valid HER-ID prefixed with OID namespace: urn:oid:2.16.578.1.12.4.1.2.{id} {$this.matches('^urn:oid:2\.16\.578\.1\.12\.4\.1\.2\.[1-9][0-9]{0,7}$')}</t>
+valid-her-id:Must be a valid HER-ID prefixed with OID namespace {$this.matches('^urn:oid:2\.16\.578\.1\.12\.4\.1\.2\.[1-9][0-9]{0,7}$')}</t>
   </si>
   <si>
     <t>MSH-25 (or MSH-6)</t>
@@ -5395,7 +5398,7 @@
         <v>39</v>
       </c>
       <c r="S37" t="s" s="2">
-        <v>39</v>
+        <v>247</v>
       </c>
       <c r="T37" t="s" s="2">
         <v>39</v>
@@ -5443,13 +5446,13 @@
         <v>39</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>39</v>
@@ -5457,7 +5460,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5480,17 +5483,17 @@
         <v>49</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>39</v>
@@ -5539,7 +5542,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5554,10 +5557,10 @@
         <v>61</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>224</v>
@@ -5565,7 +5568,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5588,19 +5591,19 @@
         <v>49</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>39</v>
@@ -5649,7 +5652,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5664,10 +5667,10 @@
         <v>61</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>224</v>
@@ -5675,7 +5678,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5698,19 +5701,19 @@
         <v>49</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>39</v>
@@ -5759,7 +5762,7 @@
         <v>39</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5774,18 +5777,18 @@
         <v>61</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5808,19 +5811,19 @@
         <v>49</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>39</v>
@@ -5869,7 +5872,7 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -5884,18 +5887,18 @@
         <v>61</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5921,14 +5924,14 @@
         <v>218</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>39</v>
@@ -5977,7 +5980,7 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>48</v>
@@ -5995,15 +5998,15 @@
         <v>39</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6109,7 +6112,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6215,7 +6218,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6321,7 +6324,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6350,11 +6353,11 @@
         <v>230</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>39</v>
@@ -6403,7 +6406,7 @@
         <v>39</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
@@ -6418,10 +6421,10 @@
         <v>61</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>39</v>
@@ -6429,7 +6432,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6455,14 +6458,14 @@
         <v>50</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>39</v>
@@ -6511,7 +6514,7 @@
         <v>39</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6526,10 +6529,10 @@
         <v>61</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>39</v>
@@ -6537,7 +6540,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6563,14 +6566,14 @@
         <v>50</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>39</v>
@@ -6619,7 +6622,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6634,10 +6637,10 @@
         <v>61</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>39</v>
@@ -6645,7 +6648,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6668,17 +6671,17 @@
         <v>49</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>39</v>
@@ -6727,7 +6730,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6742,10 +6745,10 @@
         <v>61</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>39</v>
@@ -6753,7 +6756,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6779,16 +6782,16 @@
         <v>242</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>245</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>39</v>
@@ -6837,7 +6840,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>48</v>
@@ -6852,10 +6855,10 @@
         <v>61</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>39</v>
@@ -6863,7 +6866,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6886,19 +6889,19 @@
         <v>49</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>39</v>
@@ -6947,7 +6950,7 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -6962,18 +6965,18 @@
         <v>61</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -6996,17 +6999,17 @@
         <v>49</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>39</v>
@@ -7034,10 +7037,10 @@
         <v>113</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>39</v>
@@ -7055,7 +7058,7 @@
         <v>39</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7070,18 +7073,18 @@
         <v>61</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7107,10 +7110,10 @@
         <v>218</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7161,7 +7164,7 @@
         <v>39</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>40</v>
@@ -7176,10 +7179,10 @@
         <v>61</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>39</v>
@@ -7187,7 +7190,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7293,7 +7296,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7399,7 +7402,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7505,7 +7508,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7531,14 +7534,14 @@
         <v>77</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>39</v>
@@ -7587,7 +7590,7 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>48</v>
@@ -7602,10 +7605,10 @@
         <v>61</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>39</v>
@@ -7613,7 +7616,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7639,16 +7642,16 @@
         <v>123</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>39</v>
@@ -7676,10 +7679,10 @@
         <v>144</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>39</v>
@@ -7697,7 +7700,7 @@
         <v>39</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>48</v>
@@ -7712,10 +7715,10 @@
         <v>61</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>39</v>
@@ -7723,7 +7726,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7746,19 +7749,19 @@
         <v>49</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>39</v>
@@ -7807,7 +7810,7 @@
         <v>39</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7822,10 +7825,10 @@
         <v>61</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>39</v>
@@ -7833,7 +7836,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7939,7 +7942,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8045,7 +8048,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8071,13 +8074,13 @@
         <v>50</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8127,7 +8130,7 @@
         <v>39</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8136,7 +8139,7 @@
         <v>48</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AI62" t="s" s="2">
         <v>61</v>
@@ -8153,7 +8156,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8179,13 +8182,13 @@
         <v>89</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -8214,10 +8217,10 @@
         <v>105</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="Z63" t="s" s="2">
         <v>39</v>
@@ -8235,7 +8238,7 @@
         <v>39</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8261,7 +8264,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8284,16 +8287,16 @@
         <v>49</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8343,7 +8346,7 @@
         <v>39</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
@@ -8361,7 +8364,7 @@
         <v>39</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>39</v>
@@ -8369,7 +8372,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8395,13 +8398,13 @@
         <v>50</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
@@ -8451,7 +8454,7 @@
         <v>39</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>40</v>
@@ -8477,7 +8480,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8500,19 +8503,19 @@
         <v>49</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>39</v>
@@ -8561,7 +8564,7 @@
         <v>39</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>40</v>
@@ -8579,7 +8582,7 @@
         <v>39</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>39</v>
@@ -8587,7 +8590,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8693,7 +8696,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8799,7 +8802,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8825,13 +8828,13 @@
         <v>50</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
@@ -8881,7 +8884,7 @@
         <v>39</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>40</v>
@@ -8890,7 +8893,7 @@
         <v>48</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>61</v>
@@ -8907,7 +8910,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -8933,13 +8936,13 @@
         <v>89</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
@@ -8968,10 +8971,10 @@
         <v>105</v>
       </c>
       <c r="X70" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="Y70" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>39</v>
@@ -8989,7 +8992,7 @@
         <v>39</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>40</v>
@@ -9015,7 +9018,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9038,16 +9041,16 @@
         <v>49</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
@@ -9097,7 +9100,7 @@
         <v>39</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>40</v>
@@ -9115,7 +9118,7 @@
         <v>39</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>39</v>
@@ -9123,7 +9126,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9149,13 +9152,13 @@
         <v>50</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
@@ -9205,7 +9208,7 @@
         <v>39</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>40</v>
@@ -9231,7 +9234,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9254,17 +9257,17 @@
         <v>49</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>39</v>
@@ -9313,7 +9316,7 @@
         <v>39</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>40</v>
@@ -9331,7 +9334,7 @@
         <v>39</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>39</v>

</xml_diff>

<commit_message>
MessagingCore: Json input to tests d070a2a60bd309c5d2cbfaeefe0a7f5c8610722d
</commit_message>
<xml_diff>
--- a/igs/MessagingCore/StructureDefinition-HopsMessageHeader.xlsx
+++ b/igs/MessagingCore/StructureDefinition-HopsMessageHeader.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-09-14T10:14:05+00:00</t>
+    <t>2021-09-17T11:58:41+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -894,7 +894,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-valid-her-id:Must be a valid HER-ID prefixed with OID namespace {$this.matches('^urn:oid:2\.16\.578\.1\.12\.4\.1\.2\.[1-9][0-9]{0,7}$')}</t>
+valid-her-id:Must be a valid HER-ID prefixed with OID namespace {$this.matches('^urn:oid:2\\.16\\.578\\.1\\.12\\.4\\.1\\.2\\.[1-9][0-9]{0,7}$')}</t>
   </si>
   <si>
     <t>MSH-25 (or MSH-6)</t>

</xml_diff>